<commit_message>
Integrate server interface into registration (login.js; Client)
</commit_message>
<xml_diff>
--- a/documents/command_catalog.xlsx
+++ b/documents/command_catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\ezq\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7A6C80-65FA-4EA8-8606-904D969A1EF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DCBFF0-0B9E-4934-9887-60D0B6213F07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6113" xr2:uid="{30A65A8A-5E25-429D-978C-08067F9BD356}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Modify lobby model; Implement openLobby and closeLobby
</commit_message>
<xml_diff>
--- a/documents/command_catalog.xlsx
+++ b/documents/command_catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\ezq\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15801963-B030-454A-9863-F940E15A74A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B16739-C273-4D4F-855C-84178643F16C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6113" xr2:uid="{30A65A8A-5E25-429D-978C-08067F9BD356}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Screen</t>
   </si>
@@ -68,7 +68,16 @@
     <t>Login</t>
   </si>
   <si>
-    <t>SHOW_ADMIN_SCREEN</t>
+    <t>SHOW_ACTIVE_ADMIN_SCREEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">queue, enqueueKey </t>
+  </si>
+  <si>
+    <t>SHOW_INACTIVE_ADMIN_SCREEN</t>
+  </si>
+  <si>
+    <t>enqueueKey in QR-Code einbinden</t>
   </si>
 </sst>
 </file>
@@ -463,14 +472,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -527,22 +536,26 @@
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>

</xml_diff>

<commit_message>
Implement enqueue controller and service
</commit_message>
<xml_diff>
--- a/documents/command_catalog.xlsx
+++ b/documents/command_catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\ezq\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B16739-C273-4D4F-855C-84178643F16C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC56B3D-F660-40F8-A496-34E838D2FAF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6113" xr2:uid="{30A65A8A-5E25-429D-978C-08067F9BD356}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Screen</t>
   </si>
@@ -38,9 +38,6 @@
     <t>CommandType</t>
   </si>
   <si>
-    <t>Params</t>
-  </si>
-  <si>
     <t>Registration</t>
   </si>
   <si>
@@ -71,13 +68,28 @@
     <t>SHOW_ACTIVE_ADMIN_SCREEN</t>
   </si>
   <si>
-    <t xml:space="preserve">queue, enqueueKey </t>
-  </si>
-  <si>
     <t>SHOW_INACTIVE_ADMIN_SCREEN</t>
   </si>
   <si>
-    <t>enqueueKey in QR-Code einbinden</t>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>UPDATE_OWNER_SCREEEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">queue, enqueueKey, lobbyActive </t>
+  </si>
+  <si>
+    <t>enqueueKey in QR-Code einbinden; lobbyActive for switch-button state</t>
+  </si>
+  <si>
+    <t>SHOW_USER_SUCCESSFULLY_ENQUEUED</t>
   </si>
 </sst>
 </file>
@@ -471,15 +483,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FF1B30-1EDA-48B8-9DC7-890F9728752A}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -491,28 +503,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -520,33 +532,33 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -554,9 +566,11 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -566,21 +580,35 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrate frontend and implement 'UPDATE_OWNER_SCREEN'
</commit_message>
<xml_diff>
--- a/documents/command_catalog.xlsx
+++ b/documents/command_catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\ezq\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC56B3D-F660-40F8-A496-34E838D2FAF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46B82BA-4BCE-477B-8651-64B86A1C78BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6113" xr2:uid="{30A65A8A-5E25-429D-978C-08067F9BD356}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14400" windowHeight="6113" xr2:uid="{30A65A8A-5E25-429D-978C-08067F9BD356}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Screen</t>
   </si>
@@ -65,12 +65,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>SHOW_ACTIVE_ADMIN_SCREEN</t>
-  </si>
-  <si>
-    <t>SHOW_INACTIVE_ADMIN_SCREEN</t>
-  </si>
-  <si>
     <t>Parameters</t>
   </si>
   <si>
@@ -86,10 +80,10 @@
     <t xml:space="preserve">queue, enqueueKey, lobbyActive </t>
   </si>
   <si>
-    <t>enqueueKey in QR-Code einbinden; lobbyActive for switch-button state</t>
-  </si>
-  <si>
     <t>SHOW_USER_SUCCESSFULLY_ENQUEUED</t>
+  </si>
+  <si>
+    <t>SHOW_OWNER_SCREEN</t>
   </si>
 </sst>
 </file>
@@ -135,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -158,15 +152,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -481,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FF1B30-1EDA-48B8-9DC7-890F9728752A}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -503,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -546,31 +555,27 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -581,7 +586,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -594,22 +599,46 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>